<commit_message>
update test rule definition
</commit_message>
<xml_diff>
--- a/tests/woudc-qa-rules-test1.xlsx
+++ b/tests/woudc-qa-rules-test1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="180" windowWidth="20235" windowHeight="7680"/>
+    <workbookView xWindow="120" yWindow="240" windowWidth="20235" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="qa tests" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="164">
   <si>
     <t>test_id</t>
   </si>
@@ -627,6 +627,60 @@
   </si>
   <si>
     <t>500</t>
+  </si>
+  <si>
+    <t>DM</t>
+  </si>
+  <si>
+    <t>50,55</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>FLIGHT_SUMMARY</t>
+  </si>
+  <si>
+    <t>IntegratedO3</t>
+  </si>
+  <si>
+    <t>CorrectionCode</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>ib2</t>
+  </si>
+  <si>
+    <t>0.01</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>DAILY</t>
+  </si>
+  <si>
+    <t>UTC_Begin</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>-1.6</t>
+  </si>
+  <si>
+    <t>5.0</t>
   </si>
 </sst>
 </file>
@@ -954,28 +1008,6 @@
     <cellStyle name="Normal_RWIN_Qa_Tests" xfId="1"/>
   </cellStyles>
   <dxfs count="7">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF365F91"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1062,11 +1094,33 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <bottom style="medium">
           <color rgb="FF4F81BD"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF365F91"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1079,12 +1133,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C11" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C11" totalsRowShown="0" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="5" tableBorderDxfId="3">
   <autoFilter ref="A1:C11"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Flag Value" dataDxfId="4"/>
-    <tableColumn id="2" name="Flag Name" dataDxfId="3"/>
-    <tableColumn id="3" name="Definition" dataDxfId="2"/>
+    <tableColumn id="1" name="Flag Value" dataDxfId="2"/>
+    <tableColumn id="2" name="Flag Name" dataDxfId="1"/>
+    <tableColumn id="3" name="Definition" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1377,10 +1431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X12"/>
+  <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.88671875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1539,7 +1593,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D3" s="21">
         <v>1</v>
@@ -1818,6 +1872,12 @@
       <c r="C11" s="21" t="s">
         <v>80</v>
       </c>
+      <c r="F11" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="K11" s="21" t="s">
+        <v>147</v>
+      </c>
       <c r="N11" s="21" t="s">
         <v>142</v>
       </c>
@@ -1875,6 +1935,219 @@
         <v>145</v>
       </c>
       <c r="W12" s="30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A13" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="N13" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="P13" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q13" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="R13" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="S13" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="T13" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="U13" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="W13" s="21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A14" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="N14" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="P14" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q14" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="R14" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="S14" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="T14" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="U14" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="W14" s="21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A15" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="N15" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="P15" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q15" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="R15" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="S15" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="T15" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="W15" s="21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A16" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="N16" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="P16" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q16" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="R16" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="S16" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="T16" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="U16" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="W16" s="21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A17" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="N17" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="P17" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q17" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="R17" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="S17" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="W17" s="30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A18" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="N18" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="P18" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q18" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="R18" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="S18" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="T18" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="U18" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="W18" s="21" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1889,7 +2162,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>